<commit_message>
use rijbaan_breedte but give prio to rijbaan categorie and rijstroken
</commit_message>
<xml_diff>
--- a/UploadAfschermendeConstructies/rijbanen_naar_breedte.xlsx
+++ b/UploadAfschermendeConstructies/rijbanen_naar_breedte.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$C$41</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$C$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
   <si>
     <t xml:space="preserve"> wegcategorie</t>
   </si>
@@ -43,12 +43,12 @@
     <t xml:space="preserve">rijstrook hoofdweg</t>
   </si>
   <si>
+    <t xml:space="preserve">rijstrook gewestweg</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Hoofdweg</t>
   </si>
   <si>
-    <t xml:space="preserve">rijstrook gewestweg</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Lokale weg type 1</t>
   </si>
   <si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Primaire weg II type 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Secundaire weg</t>
   </si>
   <si>
     <t xml:space="preserve"> Secundaire weg type 1</t>
@@ -204,18 +207,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:H1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -264,17 +269,15 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>930</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>640</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>310</v>
@@ -282,57 +285,57 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1010</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1380</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>1750</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2120</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>310</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -340,10 +343,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>620</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -351,10 +354,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>930</v>
+        <v>620</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -362,10 +365,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>1240</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -373,21 +376,21 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>1550</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>310</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -395,10 +398,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>620</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -406,10 +409,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>1240</v>
+        <v>620</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -417,21 +420,21 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>1550</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>310</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -439,21 +442,21 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>620</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>310</v>
+        <v>620</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -461,10 +464,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>620</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -472,32 +475,32 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>1240</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>640</v>
+        <v>930</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>1010</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -505,10 +508,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>1380</v>
+        <v>640</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -516,32 +519,32 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>1750</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>580</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>890</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -549,10 +552,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>1200</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -560,92 +563,92 @@
         <v>13</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>1510</v>
+        <v>890</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>580</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>310</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>620</v>
+        <v>580</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>930</v>
+        <v>890</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>310</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>620</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>930</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>1</v>
@@ -656,7 +659,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>2</v>
@@ -667,7 +670,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>3</v>
@@ -681,19 +684,89 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C44" s="2" t="n">
         <v>1240</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>1240</v>
+      </c>
+    </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1646,8 +1719,15 @@
     <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1006" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1007" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:C41"/>
+  <autoFilter ref="A1:C48"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>